<commit_message>
Complete unit test for the base class
</commit_message>
<xml_diff>
--- a/tests/data/expt06.xlsx
+++ b/tests/data/expt06.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Stockton university\Graduate assistantship\chemistry-experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213718B9-01FF-48B2-8A03-622976015631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9044849-DD06-4446-ADE9-C1CE420DCC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6720" yWindow="1890" windowWidth="21600" windowHeight="16020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="class data" sheetId="1" r:id="rId1"/>
+    <sheet name="class data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="complete" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Chemistry 2115:  General Chemistry Laboratory</t>
   </si>
@@ -429,7 +429,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -437,7 +437,7 @@
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -565,12 +565,6 @@
   </cellStyleXfs>
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -661,6 +655,12 @@
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -668,7 +668,6 @@
     <cellStyle name="Result2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -923,459 +922,459 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="4" customWidth="1"/>
-    <col min="3" max="6" width="18.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="18.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="4" customWidth="1"/>
     <col min="8" max="1003" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row customHeight="1" ht="18" r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row customHeight="1" ht="18" r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="1:7" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="12"/>
-      <c r="B4" s="15" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row customHeight="1" ht="18" r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row ht="34.5" r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+      <c r="B4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
-      <c r="B5" s="20">
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row customHeight="1" ht="18" r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="18">
         <v>15</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="19">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="1" t="s">
+      <c r="D5" s="20"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row customHeight="1" ht="18" r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row customHeight="1" ht="18" r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1" t="s">
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="25" t="s">
+      <c r="G7" s="35"/>
+    </row>
+    <row ht="45" r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="25" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="s">
+    <row customHeight="1" ht="18" r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-    </row>
-    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+    </row>
+    <row customHeight="1" ht="18" r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="34"/>
-    </row>
-    <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="27">
         <v>0.105</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="27">
         <v>26.718</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="27">
         <v>26.806999999999999</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-    </row>
-    <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="31" t="s">
+      <c r="E11" s="28"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="30">
         <v>0.13600000000000001</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="30">
         <v>29.81</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="30">
         <v>29.92</v>
       </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="34"/>
-    </row>
-    <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="28" t="s">
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="27">
         <v>0.122</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="27">
         <v>28.843</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="27">
         <v>28.943000000000001</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-    </row>
-    <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="31" t="s">
+      <c r="E13" s="28"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="32">
+      <c r="B14" s="30">
         <v>0.11600000000000001</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="30">
         <v>30.013999999999999</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="30">
         <v>30.106999999999999</v>
       </c>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="34"/>
-    </row>
-    <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="28" t="s">
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-    </row>
-    <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="31" t="s">
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B16" s="30">
         <v>0.161</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="30">
         <v>25.565000000000001</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="30">
         <v>25.69</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="34"/>
-    </row>
-    <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-    </row>
-    <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="31" t="s">
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="34"/>
-    </row>
-    <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="28" t="s">
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="27">
         <v>0.187</v>
       </c>
-      <c r="C19" s="29">
+      <c r="C19" s="27">
         <v>24.666</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="27">
         <v>24.802</v>
       </c>
-      <c r="E19" s="30"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-    </row>
-    <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="31" t="s">
+      <c r="E19" s="28"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="30">
         <v>0.20499999999999999</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="30">
         <v>22.372</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="30">
         <v>22.53</v>
       </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="34"/>
-    </row>
-    <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="28" t="s">
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-    </row>
-    <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="31" t="s">
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="34"/>
-    </row>
-    <row r="23" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="28" t="s">
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="29">
+      <c r="B23" s="27">
         <v>0.318</v>
       </c>
-      <c r="C23" s="29">
+      <c r="C23" s="27">
         <v>29.875</v>
       </c>
-      <c r="D23" s="29">
+      <c r="D23" s="27">
         <v>30.047000000000001</v>
       </c>
-      <c r="E23" s="30"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-    </row>
-    <row r="24" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="31" t="s">
+      <c r="E23" s="28"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="32">
+      <c r="B24" s="30">
         <v>0.25700000000000001</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="30">
         <v>30.273</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="30">
         <v>30.446000000000002</v>
       </c>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="34"/>
-    </row>
-    <row r="25" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="28" t="s">
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-    </row>
-    <row r="26" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="31" t="s">
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="34"/>
-    </row>
-    <row r="27" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="28" t="s">
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-    </row>
-    <row r="28" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="31" t="s">
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="34"/>
-    </row>
-    <row r="29" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="28" t="s">
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="29">
+      <c r="B29" s="27">
         <v>0.25</v>
       </c>
-      <c r="C29" s="29">
+      <c r="C29" s="27">
         <v>20.785</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="27">
         <v>20.962</v>
       </c>
-      <c r="E29" s="30"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-    </row>
-    <row r="30" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="31" t="s">
+      <c r="E29" s="28"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="32">
+      <c r="B30" s="30">
         <v>0.21299999999999999</v>
       </c>
-      <c r="C30" s="32">
+      <c r="C30" s="30">
         <v>22.315999999999999</v>
       </c>
-      <c r="D30" s="32">
+      <c r="D30" s="30">
         <v>22.486000000000001</v>
       </c>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="34"/>
-    </row>
-    <row r="31" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="28" t="s">
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
-    </row>
-    <row r="32" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="31" t="s">
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="32">
+      <c r="B32" s="30">
         <v>0.219</v>
       </c>
-      <c r="C32" s="32">
+      <c r="C32" s="30">
         <v>29.898</v>
       </c>
-      <c r="D32" s="32">
+      <c r="D32" s="30">
         <v>30.07</v>
       </c>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="34"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1386,7 +1385,486 @@
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="0" alignWithMargins="0">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="18.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="4" customWidth="1"/>
+    <col min="8" max="1003" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="18" r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row customHeight="1" ht="18" r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row customHeight="1" ht="18" r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row ht="34.5" r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+      <c r="B4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row customHeight="1" ht="18" r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="18">
+        <v>15</v>
+      </c>
+      <c r="C5" s="19">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D5" s="20"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row customHeight="1" ht="18" r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row customHeight="1" ht="18" r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="35"/>
+    </row>
+    <row ht="45" r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="18" r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="26">
+        <v>0.231</v>
+      </c>
+      <c r="B9" s="27">
+        <v>0.783</v>
+      </c>
+      <c r="C9" s="27">
+        <v>0.874</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+    </row>
+    <row customHeight="1" ht="18" r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="29">
+        <v>0.432</v>
+      </c>
+      <c r="B10" s="30">
+        <v>0.567</v>
+      </c>
+      <c r="C10" s="30">
+        <v>0.912</v>
+      </c>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="26">
+        <v>0.112</v>
+      </c>
+      <c r="B11" s="27">
+        <v>0.891</v>
+      </c>
+      <c r="C11" s="27">
+        <v>0.451</v>
+      </c>
+      <c r="D11" s="27">
+        <v>26.806999999999999</v>
+      </c>
+      <c r="E11" s="28"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="29">
+        <v>0.754</v>
+      </c>
+      <c r="B12" s="30">
+        <v>0.634</v>
+      </c>
+      <c r="C12" s="30">
+        <v>0.333</v>
+      </c>
+      <c r="D12" s="30">
+        <v>29.92</v>
+      </c>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="26">
+        <v>0.765</v>
+      </c>
+      <c r="B13" s="27">
+        <v>0.284</v>
+      </c>
+      <c r="C13" s="27">
+        <v>0.567</v>
+      </c>
+      <c r="D13" s="27">
+        <v>28.943000000000001</v>
+      </c>
+      <c r="E13" s="28"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="30">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="C14" s="30">
+        <v>30.013999999999999</v>
+      </c>
+      <c r="D14" s="30">
+        <v>30.106999999999999</v>
+      </c>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="30">
+        <v>0.161</v>
+      </c>
+      <c r="C16" s="30">
+        <v>25.565000000000001</v>
+      </c>
+      <c r="D16" s="30">
+        <v>25.69</v>
+      </c>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="27">
+        <v>0.187</v>
+      </c>
+      <c r="C19" s="27">
+        <v>24.666</v>
+      </c>
+      <c r="D19" s="27">
+        <v>24.802</v>
+      </c>
+      <c r="E19" s="28"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="30">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="C20" s="30">
+        <v>22.372</v>
+      </c>
+      <c r="D20" s="30">
+        <v>22.53</v>
+      </c>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="27">
+        <v>0.318</v>
+      </c>
+      <c r="C23" s="27">
+        <v>29.875</v>
+      </c>
+      <c r="D23" s="27">
+        <v>30.047000000000001</v>
+      </c>
+      <c r="E23" s="28"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="30">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="C24" s="30">
+        <v>30.273</v>
+      </c>
+      <c r="D24" s="30">
+        <v>30.446000000000002</v>
+      </c>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="27">
+        <v>0.25</v>
+      </c>
+      <c r="C29" s="27">
+        <v>20.785</v>
+      </c>
+      <c r="D29" s="27">
+        <v>20.962</v>
+      </c>
+      <c r="E29" s="28"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="30">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="C30" s="30">
+        <v>22.315999999999999</v>
+      </c>
+      <c r="D30" s="30">
+        <v>22.486000000000001</v>
+      </c>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="32"/>
+    </row>
+    <row customHeight="1" ht="18" r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+    </row>
+    <row customHeight="1" ht="18" r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="30">
+        <v>0.219</v>
+      </c>
+      <c r="C32" s="30">
+        <v>29.898</v>
+      </c>
+      <c r="D32" s="30">
+        <v>30.07</v>
+      </c>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:G7"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="0" alignWithMargins="0">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Complete all unit tests
</commit_message>
<xml_diff>
--- a/tests/data/expt06.xlsx
+++ b/tests/data/expt06.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Stockton university\Graduate assistantship\chemistry-experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Stockton university\Graduate assistantship\chemistry-experiments\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9044849-DD06-4446-ADE9-C1CE420DCC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE3823D-317A-45C9-B20D-8F41F149EF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="1890" windowWidth="21600" windowHeight="16020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13140" yWindow="3465" windowWidth="9810" windowHeight="15480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="class data" sheetId="1" state="visible" r:id="rId1"/>
@@ -1512,348 +1512,892 @@
       </c>
     </row>
     <row customHeight="1" ht="18" r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="26">
-        <v>0.231</v>
-      </c>
-      <c r="B9" s="27">
-        <v>0.783</v>
-      </c>
-      <c r="C9" s="27">
-        <v>0.874</v>
-      </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
+      <c r="A9" s="26" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="B9" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C9" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D9" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E9" s="28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F9" s="28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G9" s="28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="29">
-        <v>0.432</v>
-      </c>
-      <c r="B10" s="30">
-        <v>0.567</v>
-      </c>
-      <c r="C10" s="30">
-        <v>0.912</v>
-      </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="32"/>
+      <c r="A10" s="29" t="inlineStr">
+        <is>
+          <t>A-2</t>
+        </is>
+      </c>
+      <c r="B10" s="30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C10" s="30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D10" s="30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E10" s="31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F10" s="31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G10" s="32" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="26">
-        <v>0.112</v>
-      </c>
-      <c r="B11" s="27">
-        <v>0.891</v>
-      </c>
-      <c r="C11" s="27">
-        <v>0.451</v>
-      </c>
-      <c r="D11" s="27">
-        <v>26.806999999999999</v>
-      </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
+      <c r="A11" s="26" t="inlineStr">
+        <is>
+          <t>A-3</t>
+        </is>
+      </c>
+      <c r="B11" s="27" t="inlineStr">
+        <is>
+          <t>0.105</t>
+        </is>
+      </c>
+      <c r="C11" s="27" t="inlineStr">
+        <is>
+          <t>26.718</t>
+        </is>
+      </c>
+      <c r="D11" s="27" t="inlineStr">
+        <is>
+          <t>26.807</t>
+        </is>
+      </c>
+      <c r="E11" s="28" t="inlineStr">
+        <is>
+          <t>0.089</t>
+        </is>
+      </c>
+      <c r="F11" s="33" t="inlineStr">
+        <is>
+          <t>0.00056994</t>
+        </is>
+      </c>
+      <c r="G11" s="33" t="inlineStr">
+        <is>
+          <t>0.00060913</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="29">
-        <v>0.754</v>
-      </c>
-      <c r="B12" s="30">
-        <v>0.634</v>
-      </c>
-      <c r="C12" s="30">
-        <v>0.333</v>
-      </c>
-      <c r="D12" s="30">
-        <v>29.92</v>
-      </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="32"/>
+      <c r="A12" s="29" t="inlineStr">
+        <is>
+          <t>A-4</t>
+        </is>
+      </c>
+      <c r="B12" s="30" t="inlineStr">
+        <is>
+          <t>0.136</t>
+        </is>
+      </c>
+      <c r="C12" s="30" t="inlineStr">
+        <is>
+          <t>29.81</t>
+        </is>
+      </c>
+      <c r="D12" s="30" t="inlineStr">
+        <is>
+          <t>29.92</t>
+        </is>
+      </c>
+      <c r="E12" s="31" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="F12" s="31" t="inlineStr">
+        <is>
+          <t>0.000738208</t>
+        </is>
+      </c>
+      <c r="G12" s="32" t="inlineStr">
+        <is>
+          <t>0.000752857</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="26">
-        <v>0.765</v>
-      </c>
-      <c r="B13" s="27">
-        <v>0.284</v>
-      </c>
-      <c r="C13" s="27">
-        <v>0.567</v>
-      </c>
-      <c r="D13" s="27">
-        <v>28.943000000000001</v>
-      </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
+      <c r="A13" s="26" t="inlineStr">
+        <is>
+          <t>A-5</t>
+        </is>
+      </c>
+      <c r="B13" s="27" t="inlineStr">
+        <is>
+          <t>0.122</t>
+        </is>
+      </c>
+      <c r="C13" s="27" t="inlineStr">
+        <is>
+          <t>28.843</t>
+        </is>
+      </c>
+      <c r="D13" s="27" t="inlineStr">
+        <is>
+          <t>28.943</t>
+        </is>
+      </c>
+      <c r="E13" s="28" t="inlineStr">
+        <is>
+          <t>0.1</t>
+        </is>
+      </c>
+      <c r="F13" s="33" t="inlineStr">
+        <is>
+          <t>0.000662216</t>
+        </is>
+      </c>
+      <c r="G13" s="33" t="inlineStr">
+        <is>
+          <t>0.000684416</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="30">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="C14" s="30">
-        <v>30.013999999999999</v>
-      </c>
-      <c r="D14" s="30">
-        <v>30.106999999999999</v>
-      </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="32"/>
+      <c r="A14" s="29" t="inlineStr">
+        <is>
+          <t>A-6</t>
+        </is>
+      </c>
+      <c r="B14" s="30" t="inlineStr">
+        <is>
+          <t>0.116</t>
+        </is>
+      </c>
+      <c r="C14" s="30" t="inlineStr">
+        <is>
+          <t>30.014</t>
+        </is>
+      </c>
+      <c r="D14" s="30" t="inlineStr">
+        <is>
+          <t>30.107</t>
+        </is>
+      </c>
+      <c r="E14" s="31" t="inlineStr">
+        <is>
+          <t>0.093</t>
+        </is>
+      </c>
+      <c r="F14" s="31" t="inlineStr">
+        <is>
+          <t>0.000629648</t>
+        </is>
+      </c>
+      <c r="G14" s="32" t="inlineStr">
+        <is>
+          <t>0.000636507</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
+      <c r="A15" s="26" t="inlineStr">
+        <is>
+          <t>B-1</t>
+        </is>
+      </c>
+      <c r="B15" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C15" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D15" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E15" s="28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F15" s="33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G15" s="33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="30">
-        <v>0.161</v>
-      </c>
-      <c r="C16" s="30">
-        <v>25.565000000000001</v>
-      </c>
-      <c r="D16" s="30">
-        <v>25.69</v>
-      </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="32"/>
+      <c r="A16" s="29" t="inlineStr">
+        <is>
+          <t>B-2</t>
+        </is>
+      </c>
+      <c r="B16" s="30" t="inlineStr">
+        <is>
+          <t>0.161</t>
+        </is>
+      </c>
+      <c r="C16" s="30" t="inlineStr">
+        <is>
+          <t>25.565</t>
+        </is>
+      </c>
+      <c r="D16" s="30" t="inlineStr">
+        <is>
+          <t>25.69</t>
+        </is>
+      </c>
+      <c r="E16" s="31" t="inlineStr">
+        <is>
+          <t>0.125</t>
+        </is>
+      </c>
+      <c r="F16" s="31" t="inlineStr">
+        <is>
+          <t>0.000873908</t>
+        </is>
+      </c>
+      <c r="G16" s="32" t="inlineStr">
+        <is>
+          <t>0.00085552</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
+      <c r="A17" s="26" t="inlineStr">
+        <is>
+          <t>B-3</t>
+        </is>
+      </c>
+      <c r="B17" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C17" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D17" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E17" s="28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F17" s="33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G17" s="33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="32"/>
+      <c r="A18" s="29" t="inlineStr">
+        <is>
+          <t>B-4</t>
+        </is>
+      </c>
+      <c r="B18" s="30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C18" s="30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D18" s="30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E18" s="31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F18" s="31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G18" s="32" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="27">
-        <v>0.187</v>
-      </c>
-      <c r="C19" s="27">
-        <v>24.666</v>
-      </c>
-      <c r="D19" s="27">
-        <v>24.802</v>
-      </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
+      <c r="A19" s="26" t="inlineStr">
+        <is>
+          <t>B-5</t>
+        </is>
+      </c>
+      <c r="B19" s="27" t="inlineStr">
+        <is>
+          <t>0.187</t>
+        </is>
+      </c>
+      <c r="C19" s="27" t="inlineStr">
+        <is>
+          <t>24.666</t>
+        </is>
+      </c>
+      <c r="D19" s="27" t="inlineStr">
+        <is>
+          <t>24.802</t>
+        </is>
+      </c>
+      <c r="E19" s="28" t="inlineStr">
+        <is>
+          <t>0.136</t>
+        </is>
+      </c>
+      <c r="F19" s="33" t="inlineStr">
+        <is>
+          <t>0.001015036</t>
+        </is>
+      </c>
+      <c r="G19" s="33" t="inlineStr">
+        <is>
+          <t>0.000930806</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="30">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="C20" s="30">
-        <v>22.372</v>
-      </c>
-      <c r="D20" s="30">
-        <v>22.53</v>
-      </c>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="32"/>
+      <c r="A20" s="29" t="inlineStr">
+        <is>
+          <t>B-6</t>
+        </is>
+      </c>
+      <c r="B20" s="30" t="inlineStr">
+        <is>
+          <t>0.205</t>
+        </is>
+      </c>
+      <c r="C20" s="30" t="inlineStr">
+        <is>
+          <t>22.372</t>
+        </is>
+      </c>
+      <c r="D20" s="30" t="inlineStr">
+        <is>
+          <t>22.53</t>
+        </is>
+      </c>
+      <c r="E20" s="31" t="inlineStr">
+        <is>
+          <t>0.158</t>
+        </is>
+      </c>
+      <c r="F20" s="31" t="inlineStr">
+        <is>
+          <t>0.00111274</t>
+        </is>
+      </c>
+      <c r="G20" s="32" t="inlineStr">
+        <is>
+          <t>0.001081377</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
+      <c r="A21" s="26" t="inlineStr">
+        <is>
+          <t>C-1</t>
+        </is>
+      </c>
+      <c r="B21" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C21" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D21" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E21" s="28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F21" s="33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G21" s="33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="32"/>
+      <c r="A22" s="29" t="inlineStr">
+        <is>
+          <t>C-2</t>
+        </is>
+      </c>
+      <c r="B22" s="30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C22" s="30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D22" s="30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E22" s="31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F22" s="31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G22" s="32" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="27">
-        <v>0.318</v>
-      </c>
-      <c r="C23" s="27">
-        <v>29.875</v>
-      </c>
-      <c r="D23" s="27">
-        <v>30.047000000000001</v>
-      </c>
-      <c r="E23" s="28"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
+      <c r="A23" s="26" t="inlineStr">
+        <is>
+          <t>C-3</t>
+        </is>
+      </c>
+      <c r="B23" s="27" t="inlineStr">
+        <is>
+          <t>0.318</t>
+        </is>
+      </c>
+      <c r="C23" s="27" t="inlineStr">
+        <is>
+          <t>29.875</t>
+        </is>
+      </c>
+      <c r="D23" s="27" t="inlineStr">
+        <is>
+          <t>30.047</t>
+        </is>
+      </c>
+      <c r="E23" s="28" t="inlineStr">
+        <is>
+          <t>0.172</t>
+        </is>
+      </c>
+      <c r="F23" s="33" t="inlineStr">
+        <is>
+          <t>0.001726103</t>
+        </is>
+      </c>
+      <c r="G23" s="33" t="inlineStr">
+        <is>
+          <t>0.001177195</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="30">
-        <v>0.25700000000000001</v>
-      </c>
-      <c r="C24" s="30">
-        <v>30.273</v>
-      </c>
-      <c r="D24" s="30">
-        <v>30.446000000000002</v>
-      </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="32"/>
+      <c r="A24" s="29" t="inlineStr">
+        <is>
+          <t>C-4</t>
+        </is>
+      </c>
+      <c r="B24" s="30" t="inlineStr">
+        <is>
+          <t>0.257</t>
+        </is>
+      </c>
+      <c r="C24" s="30" t="inlineStr">
+        <is>
+          <t>30.273</t>
+        </is>
+      </c>
+      <c r="D24" s="30" t="inlineStr">
+        <is>
+          <t>30.446</t>
+        </is>
+      </c>
+      <c r="E24" s="31" t="inlineStr">
+        <is>
+          <t>0.173</t>
+        </is>
+      </c>
+      <c r="F24" s="31" t="inlineStr">
+        <is>
+          <t>0.001394995</t>
+        </is>
+      </c>
+      <c r="G24" s="32" t="inlineStr">
+        <is>
+          <t>0.001184039</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
+      <c r="A25" s="26" t="inlineStr">
+        <is>
+          <t>C-5</t>
+        </is>
+      </c>
+      <c r="B25" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C25" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D25" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E25" s="28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F25" s="33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G25" s="33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="32"/>
+      <c r="A26" s="29" t="inlineStr">
+        <is>
+          <t>C-6</t>
+        </is>
+      </c>
+      <c r="B26" s="30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C26" s="30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D26" s="30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E26" s="31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F26" s="31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G26" s="32" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
+      <c r="A27" s="26" t="inlineStr">
+        <is>
+          <t>D-1</t>
+        </is>
+      </c>
+      <c r="B27" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C27" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D27" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E27" s="28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F27" s="33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G27" s="33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="32"/>
+      <c r="A28" s="29" t="inlineStr">
+        <is>
+          <t>D-2</t>
+        </is>
+      </c>
+      <c r="B28" s="30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C28" s="30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D28" s="30" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E28" s="31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F28" s="31" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G28" s="32" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="27">
-        <v>0.25</v>
-      </c>
-      <c r="C29" s="27">
-        <v>20.785</v>
-      </c>
-      <c r="D29" s="27">
-        <v>20.962</v>
-      </c>
-      <c r="E29" s="28"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
+      <c r="A29" s="26" t="inlineStr">
+        <is>
+          <t>D-3</t>
+        </is>
+      </c>
+      <c r="B29" s="27" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="C29" s="27" t="inlineStr">
+        <is>
+          <t>20.785</t>
+        </is>
+      </c>
+      <c r="D29" s="27" t="inlineStr">
+        <is>
+          <t>20.962</t>
+        </is>
+      </c>
+      <c r="E29" s="28" t="inlineStr">
+        <is>
+          <t>0.177</t>
+        </is>
+      </c>
+      <c r="F29" s="33" t="inlineStr">
+        <is>
+          <t>0.001356999</t>
+        </is>
+      </c>
+      <c r="G29" s="33" t="inlineStr">
+        <is>
+          <t>0.001211416</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="30">
-        <v>0.21299999999999999</v>
-      </c>
-      <c r="C30" s="30">
-        <v>22.315999999999999</v>
-      </c>
-      <c r="D30" s="30">
-        <v>22.486000000000001</v>
-      </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="32"/>
+      <c r="A30" s="29" t="inlineStr">
+        <is>
+          <t>D-4</t>
+        </is>
+      </c>
+      <c r="B30" s="30" t="inlineStr">
+        <is>
+          <t>0.213</t>
+        </is>
+      </c>
+      <c r="C30" s="30" t="inlineStr">
+        <is>
+          <t>22.316</t>
+        </is>
+      </c>
+      <c r="D30" s="30" t="inlineStr">
+        <is>
+          <t>22.486</t>
+        </is>
+      </c>
+      <c r="E30" s="31" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="F30" s="31" t="inlineStr">
+        <is>
+          <t>0.001156163</t>
+        </is>
+      </c>
+      <c r="G30" s="32" t="inlineStr">
+        <is>
+          <t>0.001163507</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
+      <c r="A31" s="26" t="inlineStr">
+        <is>
+          <t>D-5</t>
+        </is>
+      </c>
+      <c r="B31" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C31" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D31" s="27" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E31" s="28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F31" s="33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G31" s="33" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="18" r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="30">
-        <v>0.219</v>
-      </c>
-      <c r="C32" s="30">
-        <v>29.898</v>
-      </c>
-      <c r="D32" s="30">
-        <v>30.07</v>
-      </c>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="32"/>
+      <c r="A32" s="29" t="inlineStr">
+        <is>
+          <t>D-6</t>
+        </is>
+      </c>
+      <c r="B32" s="30" t="inlineStr">
+        <is>
+          <t>0.219</t>
+        </is>
+      </c>
+      <c r="C32" s="30" t="inlineStr">
+        <is>
+          <t>29.898</t>
+        </is>
+      </c>
+      <c r="D32" s="30" t="inlineStr">
+        <is>
+          <t>30.07</t>
+        </is>
+      </c>
+      <c r="E32" s="31" t="inlineStr">
+        <is>
+          <t>0.172</t>
+        </is>
+      </c>
+      <c r="F32" s="31" t="inlineStr">
+        <is>
+          <t>0.001188731</t>
+        </is>
+      </c>
+      <c r="G32" s="32" t="inlineStr">
+        <is>
+          <t>0.001177195</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>